<commit_message>
File cleanup and adding comments to climate data file
</commit_message>
<xml_diff>
--- a/Papers to Revisit.xlsx
+++ b/Papers to Revisit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32940" yWindow="5140" windowWidth="20020" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Papers to Revisit.csv" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="82">
   <si>
     <t>datasetID</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>x Assume 'commercial blueberry vendor' in FL</t>
+  </si>
+  <si>
+    <t>x fixed one NA</t>
+  </si>
+  <si>
+    <t>x put in 1973, year before publication. No field chilling</t>
+  </si>
+  <si>
+    <t>For chilling unit calculations, need to pull it</t>
   </si>
 </sst>
 </file>
@@ -627,14 +636,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D67" sqref="D67"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -668,7 +676,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -685,7 +693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -725,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -736,10 +744,13 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" hidden="1">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -753,7 +764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -767,7 +778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -778,7 +789,10 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>80</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -798,7 +812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -815,7 +829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -829,7 +843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -846,7 +860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -863,7 +877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -891,7 +905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -905,7 +919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -919,7 +933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -933,7 +947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -950,7 +964,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -967,7 +981,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -984,7 +998,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -998,7 +1012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1012,7 +1026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1026,7 +1040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1057,7 +1071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1071,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1102,7 +1116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1122,7 +1136,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1133,7 +1147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1147,7 +1161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -1164,7 +1178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1178,7 +1192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1198,7 +1212,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -1212,7 +1226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1229,7 +1243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1246,7 +1260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1259,8 +1273,11 @@
       <c r="G39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" hidden="1">
+      <c r="H39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -1276,8 +1293,11 @@
       <c r="H40" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" hidden="1">
+      <c r="I40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -1291,7 +1311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -1308,7 +1328,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -1322,7 +1342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -1339,7 +1359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -1359,7 +1379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -1373,7 +1393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -1390,7 +1410,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -1421,7 +1441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -1466,7 +1486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -1480,7 +1500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -1495,16 +1515,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H54">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>